<commit_message>
Profiling completed for FRDM and BBB. Working code for both and O3 memmove function. Added Profiling Results.xlsx, that has all profiling results.
</commit_message>
<xml_diff>
--- a/Profiling Results.xlsx
+++ b/Profiling Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>memmove</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>(values in Clock Cycles)</t>
+  </si>
+  <si>
+    <t>uS</t>
   </si>
 </sst>
 </file>
@@ -489,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,17 +618,33 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>187</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1267</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12067</v>
+      </c>
+      <c r="F7" s="1">
+        <v>60067</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="I7" s="1">
+        <v>152</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1052</v>
+      </c>
+      <c r="K7" s="1">
+        <v>10052</v>
+      </c>
+      <c r="L7" s="1">
+        <v>50052</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -676,7 +695,9 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="C12" s="6">
         <v>10</v>
       </c>
@@ -689,7 +710,9 @@
       <c r="F12" s="6">
         <v>5000</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="I12" s="6">
         <v>10</v>
       </c>
@@ -707,49 +730,97 @@
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>25</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="I13" s="1">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>5</v>
+      </c>
+      <c r="L13" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1">
+        <v>128</v>
+      </c>
+      <c r="F14" s="1">
+        <v>623</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="I14" s="1">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1">
+        <v>13</v>
+      </c>
+      <c r="K14" s="1">
+        <v>94</v>
+      </c>
+      <c r="L14" s="1">
+        <v>454</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>28</v>
+      </c>
+      <c r="F15" s="1">
+        <v>122</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1">
+        <v>20</v>
+      </c>
+      <c r="L15" s="1">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
added RTC code for KL25Z , added in logging in profiler
</commit_message>
<xml_diff>
--- a/Profiling Results.xlsx
+++ b/Profiling Results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCBoulder\Acads\Sem_1\5813_Principles_of_Embedded_Software\Projects\Project3\ecen5813-Proj3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaku8856\Documents\5813-001-Proj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>memmove</t>
   </si>
@@ -44,9 +44,6 @@
     <t>BEAGLE BONE BLACK</t>
   </si>
   <si>
-    <t>(Clock Cycles)</t>
-  </si>
-  <si>
     <t>memset</t>
   </si>
   <si>
@@ -62,7 +59,7 @@
     <t>(values in Clock Cycles)</t>
   </si>
   <si>
-    <t>uS</t>
+    <t>(values in uS)</t>
   </si>
 </sst>
 </file>
@@ -165,6 +162,8 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -174,8 +173,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +490,7 @@
   <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,50 +500,50 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="H3" s="2" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6">
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
         <v>100</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>1000</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>5000</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6">
+      <c r="I4" s="3">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3">
         <v>100</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="3">
         <v>1000</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -567,7 +564,7 @@
         <v>45052</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="1">
         <v>107</v>
@@ -586,20 +583,20 @@
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>471</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>3801</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>37101</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <v>185101</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1">
         <v>397</v>
@@ -631,7 +628,7 @@
         <v>60067</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1">
         <v>152</v>
@@ -663,7 +660,7 @@
         <v>20379</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" s="1">
         <v>541</v>
@@ -679,50 +676,50 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="H11" s="2" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="H11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>100</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="3">
         <v>1000</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="3">
         <v>5000</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="H12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3">
         <v>10</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="3">
         <v>100</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="3">
         <v>1000</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -743,7 +740,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I13" s="1">
         <v>18</v>
@@ -775,7 +772,7 @@
         <v>623</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" s="1">
         <v>6</v>
@@ -807,7 +804,7 @@
         <v>122</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I15" s="1">
         <v>4</v>

</xml_diff>